<commit_message>
Cleaning and updating BOMs. Almost complete!
</commit_message>
<xml_diff>
--- a/BOM/Tube Depot dot com.xlsx
+++ b/BOM/Tube Depot dot com.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Documents/GitHub/steel-string-singer-sn-002/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339ECE74-D07A-3848-8D49-38229680FA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EEC0C5-3206-F244-BCE3-2678BCA22E4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="5180" windowWidth="28040" windowHeight="17440" xr2:uid="{E18E6AE7-4814-274C-ADCB-60CCDE6479EF}"/>
+    <workbookView xWindow="7600" yWindow="5860" windowWidth="28040" windowHeight="17440" xr2:uid="{E18E6AE7-4814-274C-ADCB-60CCDE6479EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Belton 9 Pin Miniature Chassis Mount Socket</t>
-  </si>
-  <si>
-    <t>Bulk Discount: -$1.12 x 14</t>
   </si>
   <si>
     <t>Switchcraft 3501FR RCA Jack</t>
@@ -47,13 +44,7 @@
     <t>Tin Plated Copper Buss Wire</t>
   </si>
   <si>
-    <t>Bulk Discount: -$0.02 x 10</t>
-  </si>
-  <si>
     <t>Switchcraft L12A 1/4" Jack</t>
-  </si>
-  <si>
-    <t>Switchcraft 11 1/4" Jack</t>
   </si>
   <si>
     <t>Lock Washer, Internal Tooth - 3/8"</t>
@@ -62,13 +53,7 @@
     <t>#6 Female/Female Hex Aluminum Standoff</t>
   </si>
   <si>
-    <t>Bulk Discount: -$0.17 x 40</t>
-  </si>
-  <si>
     <t>6-32 Phillips Pan Head</t>
-  </si>
-  <si>
-    <t>Bulk Discount: -$0.02 x 80</t>
   </si>
   <si>
     <t>6-32 Machine Screw Keps Nut</t>
@@ -80,31 +65,16 @@
     <t>Miniature Shield</t>
   </si>
   <si>
-    <t>Bulk Discount: -$0.12 x 14</t>
-  </si>
-  <si>
     <t>Octal Tube Clip Suitable For Fender® Brand Amplifiers</t>
-  </si>
-  <si>
-    <t>Bulk Discount: -$0.88 x 10</t>
   </si>
   <si>
     <t>18 Ga. Stranded, Tin Plated, Aerospace Grade, Tefzel Wire</t>
   </si>
   <si>
-    <t>Bulk Discount: -$0.04 x 10</t>
-  </si>
-  <si>
     <t>20 Ga. Stranded, Tin Plated, Aerospace Grade, Tefzel Wire</t>
   </si>
   <si>
-    <t>Bulk Discount: -$0.03 x 13</t>
-  </si>
-  <si>
     <t>Mogami W2524 Instrument Cable</t>
-  </si>
-  <si>
-    <t>Bulk Discount: -$0.14 x 20</t>
   </si>
   <si>
     <t>3 Lug Terminal Strip</t>
@@ -113,7 +83,40 @@
     <t>AGC Fuse Block</t>
   </si>
   <si>
-    <t>Bulk Discount: -$0.03 x 10</t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>NOR, FX Loop</t>
+  </si>
+  <si>
+    <t>FX Loop/Speaker</t>
+  </si>
+  <si>
+    <t>1/2"</t>
+  </si>
+  <si>
+    <t>3/8"</t>
+  </si>
+  <si>
+    <t>1/4"</t>
+  </si>
+  <si>
+    <t>White heater</t>
+  </si>
+  <si>
+    <t>Black heater &amp; Grounds</t>
+  </si>
+  <si>
+    <t>Red Power</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Blue</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,13 +168,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -196,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -204,11 +234,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -217,6 +243,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,8 +534,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1524000</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -551,13 +590,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -613,13 +652,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>355600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -675,13 +714,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>889000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -737,13 +776,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1524000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -799,14 +838,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>1524000</xdr:rowOff>
+      <xdr:rowOff>330200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -861,13 +900,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>330200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -923,13 +962,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>1524000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -985,13 +1024,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1524000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1047,13 +1086,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1109,13 +1148,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1171,13 +1210,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>673100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1233,14 +1272,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>292100</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1295,13 +1334,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>254000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1357,13 +1396,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>279400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1419,13 +1458,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>889000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1481,13 +1520,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1543,13 +1582,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>1524000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1605,14 +1644,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1663,26 +1702,21 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="2032000" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27"/>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D08D5B5-78B6-104B-BCEF-3C5EB14AEFF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2175F9C7-4A05-8442-BCA1-6F55203BEF8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1691,7 +1725,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1705,7 +1739,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="13627100"/>
+          <a:off x="0" y="25412700"/>
           <a:ext cx="2032000" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1724,7 +1758,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2025,779 +2059,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03272AD8-30EC-944E-A7D0-3C93CF98D3E4}">
-  <dimension ref="A3:E68"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+    <row r="1" spans="1:5" s="14" customFormat="1" ht="24">
+      <c r="A1" s="13"/>
+      <c r="D1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="12"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="10">
         <v>2.13</v>
       </c>
-      <c r="D3" s="7">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5">
-        <v>29.82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="2" t="s">
+      <c r="D3" s="11">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="124" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="17">
+      <c r="A5" s="12"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="17" thickBot="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" ht="123" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="3">
-        <v>-15.68</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C7" s="3">
         <v>2.4500000000000002</v>
       </c>
       <c r="D7" s="4">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="118" customHeight="1">
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D8" s="11">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" ht="29" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="38" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" thickBot="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" ht="128" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D8" s="7">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C12" s="3">
         <v>2.25</v>
       </c>
       <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="116" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="92" customHeight="1">
+      <c r="A14" s="9"/>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.43</v>
+      </c>
+      <c r="D14" s="11">
+        <v>40</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="50" customHeight="1">
+      <c r="A15" s="9"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" ht="19" customHeight="1">
+      <c r="A16" s="9"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1" thickBot="1">
+      <c r="A17" s="9"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9"/>
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="1" t="s">
+      <c r="C18" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D18" s="11">
+        <v>80</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17">
+      <c r="A19" s="9"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="17">
+      <c r="A20" s="9"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="87" customHeight="1" thickBot="1">
+      <c r="A21" s="9"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" ht="154" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3">
-        <v>1.95</v>
-      </c>
-      <c r="D13" s="4">
-        <v>6</v>
-      </c>
-      <c r="E13" s="3">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="116" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="1" t="s">
+      <c r="C22" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D22" s="4">
+        <v>10</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="94" customHeight="1">
+      <c r="A23" s="9"/>
+      <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C23" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="D23" s="11">
+        <v>10</v>
+      </c>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="28" customHeight="1">
+      <c r="A24" s="9"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" ht="22" customHeight="1">
+      <c r="A25" s="9"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" ht="6" customHeight="1" thickBot="1">
+      <c r="A26" s="9"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" ht="164" customHeight="1">
+      <c r="A27" s="8"/>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="122" customHeight="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="D28" s="11">
         <v>7</v>
       </c>
-      <c r="E14" s="3">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="92" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.43</v>
-      </c>
-      <c r="D15" s="7">
-        <v>40</v>
-      </c>
-      <c r="E15" s="5">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="3">
-        <v>-6.8</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="1" t="s">
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" ht="17">
+      <c r="A29" s="9"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" ht="17">
+      <c r="A30" s="9"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" ht="27" customHeight="1" thickBot="1">
+      <c r="A31" s="9"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5" ht="65" customHeight="1">
+      <c r="A32" s="9"/>
+      <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="D19" s="7">
-        <v>80</v>
-      </c>
-      <c r="E19" s="5">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="2" t="s">
+      <c r="C32" s="10">
+        <v>1.07</v>
+      </c>
+      <c r="D32" s="11">
+        <v>4</v>
+      </c>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" ht="17">
+      <c r="A33" s="9"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" ht="17">
+      <c r="A34" s="9"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" customHeight="1" thickBot="1">
+      <c r="A35" s="9"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" ht="79" customHeight="1">
+      <c r="A36" s="9"/>
+      <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="3">
-        <v>-1.6</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="154" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="1" t="s">
+      <c r="C36" s="10">
+        <v>0.41</v>
+      </c>
+      <c r="D36" s="11">
         <v>10</v>
       </c>
-      <c r="C23" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="E36" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17">
+      <c r="A37" s="9"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5" ht="17">
+      <c r="A38" s="9"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5" ht="17" thickBot="1">
+      <c r="A39" s="9"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" ht="79" customHeight="1">
+      <c r="A40" s="9"/>
+      <c r="B40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0.41</v>
+      </c>
+      <c r="D40" s="11">
+        <v>15</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17">
+      <c r="A41" s="9"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:5" ht="17">
+      <c r="A42" s="9"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" ht="17" thickBot="1">
+      <c r="A43" s="9"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="9"/>
+      <c r="B44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0.41</v>
+      </c>
+      <c r="D44" s="11">
         <v>10</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E44" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="17">
+      <c r="A45" s="9"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="1:5" ht="17">
+      <c r="A46" s="9"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:5" ht="17" thickBot="1">
+      <c r="A47" s="9"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" ht="100" customHeight="1">
+      <c r="A48" s="9"/>
+      <c r="B48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="D48" s="11">
+        <v>13</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="29" customHeight="1">
+      <c r="A49" s="9"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="1:5" ht="28" customHeight="1">
+      <c r="A50" s="9"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" ht="17" thickBot="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="1:5" ht="98" customHeight="1">
+      <c r="A52" s="9"/>
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="D52" s="11">
+        <v>13</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="23" customHeight="1">
+      <c r="A53" s="9"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" ht="17">
+      <c r="A54" s="9"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A55" s="9"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="9"/>
+      <c r="B56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="D56" s="11">
+        <v>12</v>
+      </c>
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" spans="1:5" ht="17">
+      <c r="A57" s="9"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="1:5" ht="17">
+      <c r="A58" s="9"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" ht="99" customHeight="1" thickBot="1">
+      <c r="A59" s="9"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" ht="107" customHeight="1">
+      <c r="A60" s="8"/>
+      <c r="B60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="121" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="D24" s="4">
-        <v>10</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="94" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="D25" s="7">
-        <v>10</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="164" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="D29" s="4">
-        <v>4</v>
-      </c>
-      <c r="E29" s="3">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="122" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="B30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="D30" s="7">
-        <v>14</v>
-      </c>
-      <c r="E30" s="5">
-        <v>11.62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="2" t="s">
+      <c r="D60" s="4">
+        <v>2</v>
+      </c>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" ht="148" customHeight="1">
+      <c r="A61" s="8"/>
+      <c r="B61" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-      <c r="B32" s="3">
-        <v>-1.68</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
-      <c r="B34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="5">
-        <v>1.07</v>
-      </c>
-      <c r="D34" s="7">
-        <v>10</v>
-      </c>
-      <c r="E34" s="5">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
-      <c r="B35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
-      <c r="B36" s="3">
-        <v>-8.8000000000000007</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="79" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="5">
-        <v>0.41</v>
-      </c>
-      <c r="D38" s="7">
-        <v>10</v>
-      </c>
-      <c r="E38" s="5">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="3">
-        <v>-0.4</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="5">
-        <v>0.41</v>
-      </c>
-      <c r="D42" s="7">
-        <v>10</v>
-      </c>
-      <c r="E42" s="5">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
-      <c r="B44" s="3">
-        <v>-0.4</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D46" s="4">
-        <v>7</v>
-      </c>
-      <c r="E46" s="3">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11"/>
-      <c r="B47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="5">
-        <v>0.37</v>
-      </c>
-      <c r="D47" s="7">
-        <v>13</v>
-      </c>
-      <c r="E47" s="5">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11"/>
-      <c r="B48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="3">
-        <v>-0.39</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11"/>
-      <c r="B51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="5">
-        <v>0.37</v>
-      </c>
-      <c r="D51" s="7">
-        <v>13</v>
-      </c>
-      <c r="E51" s="5">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11"/>
-      <c r="B52" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="11"/>
-      <c r="B53" s="3">
-        <v>-0.39</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="11"/>
-      <c r="B55" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="D55" s="7">
-        <v>20</v>
-      </c>
-      <c r="E55" s="5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="11"/>
-      <c r="B56" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="11"/>
-      <c r="B57" s="3">
-        <v>-2.8</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5" ht="107" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="10"/>
-      <c r="B59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D59" s="4">
-        <v>2</v>
-      </c>
-      <c r="E59" s="3">
+      <c r="C61" s="3">
+        <v>3.95</v>
+      </c>
+      <c r="D61" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="148" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="10"/>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="3">
-        <v>3.95</v>
-      </c>
-      <c r="D60" s="4">
-        <v>1</v>
-      </c>
-      <c r="E60" s="3">
-        <v>3.95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="11"/>
-      <c r="B61" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61" s="5">
-        <v>0.41</v>
-      </c>
-      <c r="D61" s="7">
-        <v>10</v>
-      </c>
-      <c r="E61" s="5">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="11"/>
-      <c r="B62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="11"/>
-      <c r="B63" s="3">
-        <v>-0.4</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="11"/>
-      <c r="B65" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" s="5">
-        <v>0.37</v>
-      </c>
-      <c r="D65" s="7">
-        <v>10</v>
-      </c>
-      <c r="E65" s="5">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="11"/>
-      <c r="B66" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="11"/>
-      <c r="B67" s="3">
-        <v>-0.3</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="5"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
+  <mergeCells count="52">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D3:D6"/>
@@ -2806,34 +2697,74 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="E8:E11"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="E56:E59"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://tubedepot.com/products/belton-9-pin-miniature-chassis-mount-socket" xr:uid="{6EFD0DFC-20E9-5B40-BB0E-A5D1D90F14D6}"/>
     <hyperlink ref="B7" r:id="rId2" display="https://tubedepot.com/products/switchcraft-3501fr-rca-jack" xr:uid="{A404F1CD-752D-7346-B2C7-1D6803DF9DA3}"/>
     <hyperlink ref="B8" r:id="rId3" display="https://tubedepot.com/products/tin-plated-copper-buss-wire" xr:uid="{01A6ED11-2DFD-D248-A5E5-065CD5529A76}"/>
     <hyperlink ref="B12" r:id="rId4" display="https://tubedepot.com/products/switchcraft-l12a-1-4-jack" xr:uid="{9D58D440-5994-8E42-8AF5-3F65F7259E76}"/>
-    <hyperlink ref="B13" r:id="rId5" display="https://tubedepot.com/products/switchcraft-11-1-4-jack" xr:uid="{B33D841A-047E-D844-818A-27159805DFC0}"/>
-    <hyperlink ref="B14" r:id="rId6" display="https://tubedepot.com/products/lock-washer-internal-tooth-3-8" xr:uid="{2662E4D9-3E99-F34C-BB0A-979DBD8E6642}"/>
-    <hyperlink ref="B15" r:id="rId7" display="https://tubedepot.com/products/number-6-female-female-hex-aluminum-standoff" xr:uid="{82DA4FFB-91DB-334F-A1F0-9BC29A1713C7}"/>
-    <hyperlink ref="B19" r:id="rId8" display="https://tubedepot.com/products/6-32-phillips-pan-head" xr:uid="{BC78D543-38C1-4A41-8C88-64BB1BB73FF6}"/>
-    <hyperlink ref="B23" r:id="rId9" display="https://tubedepot.com/products/6-32-phillips-pan-head" xr:uid="{6AA8AAFD-8063-C34C-A2E5-11212D79F61B}"/>
-    <hyperlink ref="B24" r:id="rId10" display="https://tubedepot.com/products/6-32-phillips-pan-head" xr:uid="{7E590D10-25B9-2F4F-BF46-5D889359D757}"/>
-    <hyperlink ref="B25" r:id="rId11" display="https://tubedepot.com/products/6-32-machine-screw-keps-nut" xr:uid="{62403DBD-435C-2C49-A287-8C0C285C402F}"/>
-    <hyperlink ref="B29" r:id="rId12" display="https://tubedepot.com/products/5-lug-terminal-strip" xr:uid="{A333B77F-A74B-A240-B4F6-CDB33096A1B3}"/>
-    <hyperlink ref="B30" r:id="rId13" display="https://tubedepot.com/products/miniature-shield" xr:uid="{19E1C693-2A7D-0E44-AA41-B5BA2B74536F}"/>
-    <hyperlink ref="B34" r:id="rId14" display="https://tubedepot.com/products/octal-tube-clip-as-used-in-fender-amps" xr:uid="{F451AD3D-0059-7240-BD1D-23761D8FAB44}"/>
-    <hyperlink ref="B38" r:id="rId15" display="https://tubedepot.com/products/18-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{CD7CAA16-5D67-2046-9D7F-CD1431F5FEFE}"/>
-    <hyperlink ref="B42" r:id="rId16" display="https://tubedepot.com/products/18-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{111E3FBA-5036-BF4F-BA6A-82F6D517DA5A}"/>
-    <hyperlink ref="B46" r:id="rId17" display="https://tubedepot.com/products/20-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{1A0262CA-F243-6E46-B990-B157FB63FA60}"/>
-    <hyperlink ref="B47" r:id="rId18" display="https://tubedepot.com/products/20-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{DE300263-D3B0-144E-8A8D-7324537EBD7F}"/>
-    <hyperlink ref="B51" r:id="rId19" display="https://tubedepot.com/products/20-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{A64BC2BB-7FD7-7042-A6E7-BCF06786EA6A}"/>
-    <hyperlink ref="B55" r:id="rId20" display="https://tubedepot.com/products/mogami-w2524-instrument-cable" xr:uid="{9C586264-AE0A-5243-8103-C532F1DA8548}"/>
-    <hyperlink ref="B59" r:id="rId21" display="https://tubedepot.com/products/3-lug-terminal-strip" xr:uid="{6ABF82DE-492B-E14A-823D-5F364407B6EC}"/>
-    <hyperlink ref="B60" r:id="rId22" display="https://tubedepot.com/products/agc-fuse-block" xr:uid="{2700C269-C3A9-7A4B-804D-C1B65033C918}"/>
-    <hyperlink ref="B61" r:id="rId23" display="https://tubedepot.com/products/18-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{706B78E3-82F9-1C4D-87CB-36A0FE2B08F5}"/>
-    <hyperlink ref="B65" r:id="rId24" display="https://tubedepot.com/products/20-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{1E37CCF2-38EE-1F43-BBA9-EE17589EFB7B}"/>
+    <hyperlink ref="B13" r:id="rId5" display="https://tubedepot.com/products/lock-washer-internal-tooth-3-8" xr:uid="{2662E4D9-3E99-F34C-BB0A-979DBD8E6642}"/>
+    <hyperlink ref="B14" r:id="rId6" display="https://tubedepot.com/products/number-6-female-female-hex-aluminum-standoff" xr:uid="{82DA4FFB-91DB-334F-A1F0-9BC29A1713C7}"/>
+    <hyperlink ref="B18" r:id="rId7" display="https://tubedepot.com/products/6-32-phillips-pan-head" xr:uid="{BC78D543-38C1-4A41-8C88-64BB1BB73FF6}"/>
+    <hyperlink ref="B22" r:id="rId8" display="https://tubedepot.com/products/6-32-phillips-pan-head" xr:uid="{6AA8AAFD-8063-C34C-A2E5-11212D79F61B}"/>
+    <hyperlink ref="B23" r:id="rId9" display="https://tubedepot.com/products/6-32-machine-screw-keps-nut" xr:uid="{62403DBD-435C-2C49-A287-8C0C285C402F}"/>
+    <hyperlink ref="B27" r:id="rId10" display="https://tubedepot.com/products/5-lug-terminal-strip" xr:uid="{A333B77F-A74B-A240-B4F6-CDB33096A1B3}"/>
+    <hyperlink ref="B28" r:id="rId11" display="https://tubedepot.com/products/miniature-shield" xr:uid="{19E1C693-2A7D-0E44-AA41-B5BA2B74536F}"/>
+    <hyperlink ref="B32" r:id="rId12" display="https://tubedepot.com/products/octal-tube-clip-as-used-in-fender-amps" xr:uid="{F451AD3D-0059-7240-BD1D-23761D8FAB44}"/>
+    <hyperlink ref="B40" r:id="rId13" display="https://tubedepot.com/products/18-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{CD7CAA16-5D67-2046-9D7F-CD1431F5FEFE}"/>
+    <hyperlink ref="B44" r:id="rId14" display="https://tubedepot.com/products/18-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{111E3FBA-5036-BF4F-BA6A-82F6D517DA5A}"/>
+    <hyperlink ref="B48" r:id="rId15" display="https://tubedepot.com/products/20-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{DE300263-D3B0-144E-8A8D-7324537EBD7F}"/>
+    <hyperlink ref="B52" r:id="rId16" display="https://tubedepot.com/products/20-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{A64BC2BB-7FD7-7042-A6E7-BCF06786EA6A}"/>
+    <hyperlink ref="B56" r:id="rId17" display="https://tubedepot.com/products/mogami-w2524-instrument-cable" xr:uid="{9C586264-AE0A-5243-8103-C532F1DA8548}"/>
+    <hyperlink ref="B60" r:id="rId18" display="https://tubedepot.com/products/3-lug-terminal-strip" xr:uid="{6ABF82DE-492B-E14A-823D-5F364407B6EC}"/>
+    <hyperlink ref="B61" r:id="rId19" display="https://tubedepot.com/products/agc-fuse-block" xr:uid="{2700C269-C3A9-7A4B-804D-C1B65033C918}"/>
+    <hyperlink ref="B36" r:id="rId20" display="https://tubedepot.com/products/18-ga-tin-plated-aerospace-grade-tefzel-wire" xr:uid="{43DB747F-1D4C-6A4A-9AEA-26D001DB2075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId25"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>